<commit_message>
[IMP] test data upgrade
</commit_message>
<xml_diff>
--- a/z0bug_odoo/z0bug_odoo/data/account_invoice_line.xlsx
+++ b/z0bug_odoo/z0bug_odoo/data/account_invoice_line.xlsx
@@ -995,11 +995,11 @@
   <dimension ref="A1:N63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E42" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
-      <selection pane="bottomRight" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+      <selection pane="bottomRight" activeCell="Q45" activeCellId="0" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2310,6 +2310,9 @@
         <v>20</v>
       </c>
       <c r="J45" s="3"/>
+      <c r="K45" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">

</xml_diff>